<commit_message>
tune bmd33 heuristic weights, add pic and comments
</commit_message>
<xml_diff>
--- a/Project 5/Results.xlsx
+++ b/Project 5/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://calvincollege-my.sharepoint.com/personal/bmd33_calvin_edu/Documents/Classes/CS 212/CS_212_Projects/Project 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28120741-49F6-4698-BB74-34074510C9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{28120741-49F6-4698-BB74-34074510C9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9639416D-9433-4875-AD9C-DBEC426D06CF}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="-108" windowWidth="22200" windowHeight="13176" xr2:uid="{3E50306C-DEB8-446C-95BB-15DDBBCC2B48}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{3E50306C-DEB8-446C-95BB-15DDBBCC2B48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>Time Limit</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Opponent</t>
   </si>
   <si>
-    <t>Bonzo</t>
-  </si>
-  <si>
     <t>currentScoreWeight</t>
   </si>
   <si>
@@ -64,13 +61,34 @@
   </si>
   <si>
     <t>Gabi</t>
+  </si>
+  <si>
+    <t>vs dfs</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>AlphaBeta</t>
+  </si>
+  <si>
+    <t>Player Score</t>
+  </si>
+  <si>
+    <t>Opponent Score</t>
+  </si>
+  <si>
+    <t>(Same heuristic, should be equal)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +100,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,9 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,61 +459,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D581CA1-FC8F-4A6E-BE70-A974D8834ED6}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -487,321 +527,471 @@
         <v>1</v>
       </c>
       <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
         <v>1000</v>
       </c>
-      <c r="G2">
-        <v>45</v>
-      </c>
       <c r="H2">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I2">
-        <f>G2-H2</f>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <f>H2-I2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
         <v>1000</v>
       </c>
-      <c r="G3">
-        <v>55</v>
-      </c>
       <c r="H3">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I30" si="0">G3-H3</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J30" si="0">H3-I3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>10</v>
+      <c r="E4" s="1">
+        <v>5</v>
       </c>
       <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>1000</v>
       </c>
-      <c r="G4">
-        <v>55</v>
-      </c>
       <c r="H4">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>10</v>
+      <c r="E5" s="1">
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>51</v>
+        <v>1000</v>
       </c>
       <c r="H5">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="2">
+        <v>50</v>
+      </c>
+      <c r="I6" s="2">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>35</v>
+      </c>
+      <c r="I7" s="2">
+        <v>61</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>59</v>
+      </c>
+      <c r="I8" s="2">
+        <v>37</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="F6">
-        <v>1000</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="E9" s="3">
         <v>3</v>
       </c>
-      <c r="F7">
-        <v>1000</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>1000</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>1000</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>1000</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>66</v>
+      </c>
+      <c r="I9" s="2">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4000</v>
+      </c>
+      <c r="H10" s="2">
+        <v>67</v>
+      </c>
+      <c r="I10" s="2">
+        <v>29</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>58</v>
+      </c>
+      <c r="I11" s="2">
+        <v>38</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>9</v>
       </c>
-      <c r="B34">
-        <v>10</v>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34">
         <v>1000</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>72</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>24</v>
       </c>
-      <c r="I34">
-        <f>G34-H34</f>
+      <c r="J34">
+        <f>H34-I34</f>
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I33 I35:I1048576">
+  <conditionalFormatting sqref="J1:J33 J35:J1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>